<commit_message>
Some intermediate commits to preserve updates to transformations and, new outputs in energy, and some minor improvements.
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_ip_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_ip_demo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D0B2E6-E55D-B245-84DB-715B5504F4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE66417-8063-D241-9BA6-0C7BA9DBCA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9540" yWindow="500" windowWidth="22160" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,7 +1060,7 @@
   <dimension ref="A1:AS158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated energy templates to fix minor missing stratgegy bug. Intermediate code pushes for transformation work in AFOLU.
</commit_message>
<xml_diff>
--- a/ref/ingestion/demo/model_input_variables_ip_demo.xlsx
+++ b/ref/ingestion/demo/model_input_variables_ip_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB07DE9B-2E44-9643-BD15-2F5659FDC4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A41EC2F-A055-6048-B138-9EAA57160A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="500" windowWidth="22160" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17180" yWindow="2440" windowWidth="22160" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="K181" sqref="K181"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>